<commit_message>
perf(devops): save profile correctly V
</commit_message>
<xml_diff>
--- a/swipeFileSep.xlsx
+++ b/swipeFileSep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Dev/yunazon-learn-browser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2856DE5-94C6-CA41-BB6A-3B4CA4868795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D347B493-B1BB-9D45-91E2-B7EDC07BB878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{64A1BDBE-28CC-D24C-801E-775E35A26A2B}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="54">
   <si>
     <t>loginSource</t>
   </si>
@@ -567,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70C5B93-5231-084F-98E7-BBB3047BCD91}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1434,6 +1434,31 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
+    <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="4" t="b">
+        <f t="shared" ref="F32" si="12">A32=D32</f>
+        <v>1</v>
+      </c>
+      <c r="G32" s="4" t="b">
+        <f t="shared" ref="G32" si="13">B32=E32</f>
+        <v>1</v>
+      </c>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
perf(devops): add basic async loading readUsers
</commit_message>
<xml_diff>
--- a/swipeFileSep.xlsx
+++ b/swipeFileSep.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Dev/yunazon-learn-browser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D347B493-B1BB-9D45-91E2-B7EDC07BB878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD2F8A9-9DB0-0940-9B62-4269F77D09F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{64A1BDBE-28CC-D24C-801E-775E35A26A2B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{64A1BDBE-28CC-D24C-801E-775E35A26A2B}"/>
   </bookViews>
   <sheets>
     <sheet name="UserModel" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="72">
   <si>
     <t>loginSource</t>
   </si>
@@ -194,6 +195,60 @@
   </si>
   <si>
     <t>userIdAuth</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>En</t>
+  </si>
+  <si>
+    <t>En, Ch</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test2</t>
   </si>
 </sst>
 </file>
@@ -569,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70C5B93-5231-084F-98E7-BBB3047BCD91}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1462,4 +1517,122 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF047898-5720-3749-9A60-B1FDAA6F2976}">
+  <dimension ref="A4:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
perf(devops): add basic async loading readUsers IV
</commit_message>
<xml_diff>
--- a/swipeFileSep.xlsx
+++ b/swipeFileSep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Dev/yunazon-learn-browser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD2F8A9-9DB0-0940-9B62-4269F77D09F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF37880-92AA-A544-B739-FFA4D3298FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{64A1BDBE-28CC-D24C-801E-775E35A26A2B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="73">
   <si>
     <t>loginSource</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Test2</t>
+  </si>
+  <si>
+    <t>YearBirth</t>
   </si>
 </sst>
 </file>
@@ -1521,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF047898-5720-3749-9A60-B1FDAA6F2976}">
-  <dimension ref="A4:D11"/>
+  <dimension ref="A4:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1620,15 +1623,29 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11">
+        <v>1990</v>
+      </c>
+      <c r="C11">
+        <v>1995</v>
+      </c>
+      <c r="D11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>62</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>69</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
perf(devops): dev profile matrix, plate VI
</commit_message>
<xml_diff>
--- a/swipeFileSep.xlsx
+++ b/swipeFileSep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Dev/yunazon-learn-browser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF37880-92AA-A544-B739-FFA4D3298FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222C114A-F625-3D49-BF22-64EB7B3ED209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{64A1BDBE-28CC-D24C-801E-775E35A26A2B}"/>
   </bookViews>
@@ -1527,7 +1527,7 @@
   <dimension ref="A4:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>